<commit_message>
standardise test files and update overview
</commit_message>
<xml_diff>
--- a/resources/tests/Test Overview.xlsx
+++ b/resources/tests/Test Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT projects\Uni\Advanced Programming\APT_A2\resources\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37403C-EC9A-49A8-8685-EF700A85812B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81632366-2A0D-4028-B5FB-BDCB20A0B63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FF8F862-1698-46C6-9AEF-8E570B750E0D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>Test Cases</t>
   </si>
@@ -267,6 +267,93 @@
   </si>
   <si>
     <t>Diff Command</t>
+  </si>
+  <si>
+    <t>End Round Scoring</t>
+  </si>
+  <si>
+    <t>End Game Scoring</t>
+  </si>
+  <si>
+    <t>ERS-1</t>
+  </si>
+  <si>
+    <t>EGS-1</t>
+  </si>
+  <si>
+    <t>Player 1 has a tile move across that has 2 horizontally adjacent, none vertically ajacent. They have 0 on broken.</t>
+  </si>
+  <si>
+    <t>ERS-2</t>
+  </si>
+  <si>
+    <t>ERS-3</t>
+  </si>
+  <si>
+    <t>Player 1 has a tile move across that has 2 horizontally adjacent, 3 vertically ajacent. They have 0 on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's score increases by 7.</t>
+  </si>
+  <si>
+    <t>Player 1's score increases by 3.</t>
+  </si>
+  <si>
+    <t>Player 1 has a score of 10, and move 0 tiles to the mosaic at the end of round. They have 2 tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's score decreases by 2 resulting in a score of 8.</t>
+  </si>
+  <si>
+    <t>ERS-4</t>
+  </si>
+  <si>
+    <t>Player 1 has a score of 10, and move 0 tiles to the mosaic at the end of round. They have 5 tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's score decreases by 8 resulting in a score of 2.</t>
+  </si>
+  <si>
+    <t>ERS-5</t>
+  </si>
+  <si>
+    <t>Player 1 has a score of 10, and move 0 tiles to the mosaic at the end of round. They have 6 tiles on broken.</t>
+  </si>
+  <si>
+    <t>ERS-6</t>
+  </si>
+  <si>
+    <t>Player 1 has a score of 12, and move 0 tiles to the mosaic at the end of round. They have 6 tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's score decreases by 11 resulting in a score of 1.</t>
+  </si>
+  <si>
+    <t>Player 1's loses 11 points but scores cannot go below zero, resulting in a score of 0.</t>
+  </si>
+  <si>
+    <t>EGS-2</t>
+  </si>
+  <si>
+    <t>EGS-3</t>
+  </si>
+  <si>
+    <t>Player 1's score is 10. Player 1 completes a row with all factories empty and no other completed tiles on their mosaic. No tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's score is 10. Player 1 completes a row with all factories empty and one column completed on their mosaic (not near the final tile). No tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's final score is 17 (5 for completing a row creating 5 adjacent tiles, and 2 for end of game points - 2 per row completed)</t>
+  </si>
+  <si>
+    <t>Player 1's final score is 24 (5 for completing a row creating 5 adjacent tiles, and 9 for end of game points - 2 per row completed &amp; 7 per column completed)</t>
+  </si>
+  <si>
+    <t>Player 1's score is 10. Player 1 places tile 'L' to complete the top row with all factories empty and have also completed all tiles on the mosaic of colour R. No tiles on broken.</t>
+  </si>
+  <si>
+    <t>Player 1's final score is 27 (5 for completing a row creating 5 adjacent tiles, and 12 for end of game points - 2 per row completed * 10 per all 5 tiles of same colour completed).</t>
   </si>
 </sst>
 </file>
@@ -373,17 +460,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -520,6 +596,17 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -551,19 +638,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E8338C1-B0E6-4AC6-B59E-C4857EED61F2}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
-  <autoFilter ref="A1:J29" xr:uid="{1C8E9E65-CE6B-4183-A98A-CD27BC43D491}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E8338C1-B0E6-4AC6-B59E-C4857EED61F2}" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J31" xr:uid="{1C8E9E65-CE6B-4183-A98A-CD27BC43D491}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3D5E04B3-7394-498A-BE20-0F63775B1FC0}" name="Column1" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{76961F5D-265B-445C-9B4C-82CDEC9BE9F3}" name="Column2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{6490194D-7D40-420A-8881-E6079B324E13}" name="Column3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{ADFBBFF3-78B8-4B98-AE69-2170ED885286}" name="Column4" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{C54A4BDB-C460-4E1D-955D-CBF7AC4ADD11}" name="Column5" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{9FA6A9EF-57BE-47E8-BED8-D9B37C8F6ACF}" name="Column6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{36097D4A-A020-4457-BF1C-FEBED2165472}" name="Column7" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{1A41BC59-BD08-485F-A2B0-66EF11DDD67A}" name="Column73" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{6848FF34-43EB-4906-947D-40C31A5ED963}" name="Column72" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{8DE37288-FFA5-4FB3-B7EA-61ABA8E9A543}" name="Column8" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3D5E04B3-7394-498A-BE20-0F63775B1FC0}" name="Column1" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{76961F5D-265B-445C-9B4C-82CDEC9BE9F3}" name="Column2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6490194D-7D40-420A-8881-E6079B324E13}" name="Column3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{ADFBBFF3-78B8-4B98-AE69-2170ED885286}" name="Column4" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{C54A4BDB-C460-4E1D-955D-CBF7AC4ADD11}" name="Column5" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{9FA6A9EF-57BE-47E8-BED8-D9B37C8F6ACF}" name="Column6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{36097D4A-A020-4457-BF1C-FEBED2165472}" name="Column7" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{1A41BC59-BD08-485F-A2B0-66EF11DDD67A}" name="Column73" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{6848FF34-43EB-4906-947D-40C31A5ED963}" name="Column72" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{8DE37288-FFA5-4FB3-B7EA-61ABA8E9A543}" name="Column8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -866,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729E1B14-47AD-493D-8C49-9EC00A8292CA}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,11 +1350,19 @@
       <c r="I18" s="9"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
+    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
       <c r="G19" s="9"/>
@@ -1275,11 +1370,19 @@
       <c r="I19" s="9"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="6"/>
       <c r="G20" s="9"/>
@@ -1287,11 +1390,19 @@
       <c r="I20" s="9"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="6"/>
       <c r="G21" s="9"/>
@@ -1299,11 +1410,19 @@
       <c r="I21" s="9"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
+    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="6"/>
       <c r="G22" s="9"/>
@@ -1311,11 +1430,19 @@
       <c r="I22" s="9"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="6"/>
+    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="6"/>
       <c r="G23" s="9"/>
@@ -1323,11 +1450,19 @@
       <c r="I23" s="9"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
+    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="6"/>
       <c r="G24" s="9"/>
@@ -1335,11 +1470,19 @@
       <c r="I24" s="9"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
+    <row r="25" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
@@ -1347,58 +1490,58 @@
       <c r="I25" s="9"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>67</v>
+    <row r="26" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="7"/>
       <c r="F26" s="6"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>20</v>
+    <row r="27" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="7"/>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="6"/>
@@ -1409,16 +1552,16 @@
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>66</v>
+        <v>21</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="6"/>
@@ -1426,6 +1569,46 @@
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
all test cases finalized.
</commit_message>
<xml_diff>
--- a/resources/tests/Test Overview.xlsx
+++ b/resources/tests/Test Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT projects\Uni\Advanced Programming\APT_A2\resources\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moditha/APT/APT_A2/resources/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81632366-2A0D-4028-B5FB-BDCB20A0B63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1847A16-DA57-9144-BC29-673047850423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FF8F862-1698-46C6-9AEF-8E570B750E0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0FF8F862-1698-46C6-9AEF-8E570B750E0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="153">
   <si>
     <t>Test Cases</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Pick a single tile from factory 4 and attempt to place on storage 1 when mosaic row 1 is already completed for that colour.</t>
   </si>
   <si>
-    <t>Pick a single tile from factory 1 and attempt to place on a full broken row.</t>
-  </si>
-  <si>
     <t>Tile will be added to the box lid instead of to the broken row.</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>Pick 1 'B' tile from factory 5 and place on storage 5.</t>
   </si>
   <si>
-    <t>Pick 1 'Y' tile from centre factory and place on storage 3.</t>
-  </si>
-  <si>
-    <t>Pick 1 'L' tile from factory 3 and place on "broken" (aka. Floor).</t>
-  </si>
-  <si>
     <t>Pick 1 'U' tile from factory 2 and attempt to place on full (of tile 'U') storage row 1.</t>
   </si>
   <si>
@@ -158,12 +149,6 @@
     <t>The 'B' tile will be placed on storage row 5.</t>
   </si>
   <si>
-    <t>The 'Y' tile will be placed on storage row 3.</t>
-  </si>
-  <si>
-    <t>The 'L' tile will be placed on the broken row.</t>
-  </si>
-  <si>
     <t>The game state will not change as this move is not allowed.</t>
   </si>
   <si>
@@ -354,15 +339,178 @@
   </si>
   <si>
     <t>Player 1's final score is 27 (5 for completing a row creating 5 adjacent tiles, and 12 for end of game points - 2 per row completed * 10 per all 5 tiles of same colour completed).</t>
+  </si>
+  <si>
+    <t>Pick 1 'B' tile from centre factory and place on storage 2.</t>
+  </si>
+  <si>
+    <t>The 'B' tile will be placed on storage row 2.</t>
+  </si>
+  <si>
+    <t>Pick 2 'B' tile from factory 2 and place on "broken" (aka. Floor).</t>
+  </si>
+  <si>
+    <t>The 'B' tiles will be placed on the broken row.</t>
+  </si>
+  <si>
+    <t>TP9_input.txt</t>
+  </si>
+  <si>
+    <t>TP9_expected.txt</t>
+  </si>
+  <si>
+    <t>UI1_expected.txt</t>
+  </si>
+  <si>
+    <t>UI1_input.txt</t>
+  </si>
+  <si>
+    <t>UI2_input.txt</t>
+  </si>
+  <si>
+    <t>UI2_expected.txt</t>
+  </si>
+  <si>
+    <t>UI3_input.txt</t>
+  </si>
+  <si>
+    <t>UI4_input.txt</t>
+  </si>
+  <si>
+    <t>UI5_input.txt</t>
+  </si>
+  <si>
+    <t>UI5_expected.txt</t>
+  </si>
+  <si>
+    <t>UI6_expected.txt</t>
+  </si>
+  <si>
+    <t>UI6_input.txt</t>
+  </si>
+  <si>
+    <t>TP1_input.txt</t>
+  </si>
+  <si>
+    <t>ESR1_input.txt</t>
+  </si>
+  <si>
+    <t>UI3_expected.txt</t>
+  </si>
+  <si>
+    <t>UI4_expected.txt</t>
+  </si>
+  <si>
+    <t>TP1_expected.txt</t>
+  </si>
+  <si>
+    <t>TP2_input.txt</t>
+  </si>
+  <si>
+    <t>TP2_expected.txt</t>
+  </si>
+  <si>
+    <t>TP3_input.txt</t>
+  </si>
+  <si>
+    <t>TP3_expected.txt</t>
+  </si>
+  <si>
+    <t>TP4_input.txt</t>
+  </si>
+  <si>
+    <t>TP4_expected.txt</t>
+  </si>
+  <si>
+    <t>TP5_input.txt</t>
+  </si>
+  <si>
+    <t>TP5_expected.txt</t>
+  </si>
+  <si>
+    <t>TP6_input.txt</t>
+  </si>
+  <si>
+    <t>TP6_expected.txt</t>
+  </si>
+  <si>
+    <t>TP7_input.txt</t>
+  </si>
+  <si>
+    <t>TP7_expected.txt</t>
+  </si>
+  <si>
+    <t>TP8_input.txt</t>
+  </si>
+  <si>
+    <t>TP8_expected.txt</t>
+  </si>
+  <si>
+    <t>RS1_input.txt</t>
+  </si>
+  <si>
+    <t>LS1_input.txt</t>
+  </si>
+  <si>
+    <t>TS1_input.txt</t>
+  </si>
+  <si>
+    <t>RS1_expected.txt</t>
+  </si>
+  <si>
+    <t>LS1_expected.txt</t>
+  </si>
+  <si>
+    <t>TS1_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR1_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR2_input.txt</t>
+  </si>
+  <si>
+    <t>ESR3_input.txt</t>
+  </si>
+  <si>
+    <t>ESR4_input.txt</t>
+  </si>
+  <si>
+    <t>ESR5_input.txt</t>
+  </si>
+  <si>
+    <t>ESR6_input.txt</t>
+  </si>
+  <si>
+    <t>ESR2_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR3_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR4_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR5_expected.txt</t>
+  </si>
+  <si>
+    <t>ESR6_expected.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -426,34 +574,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,24 +1109,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729E1B14-47AD-493D-8C49-9EC00A8292CA}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.5" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -995,16 +1149,16 @@
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1172,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1026,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>
@@ -1041,16 +1195,16 @@
         <v>11</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1058,19 +1212,23 @@
         <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1078,19 +1236,23 @@
         <v>17</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1098,19 +1260,23 @@
         <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="10" t="s">
+        <v>125</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1118,19 +1284,23 @@
         <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>103</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="10" t="s">
+        <v>127</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1138,19 +1308,23 @@
         <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1161,16 +1335,20 @@
         <v>24</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1181,307 +1359,367 @@
         <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="10" t="s">
+        <v>133</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="8">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>134</v>
+      </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>108</v>
+      </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="10" t="s">
+        <v>107</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="10" t="s">
+        <v>110</v>
+      </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>111</v>
+      </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="10" t="s">
+        <v>119</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="C16" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>112</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="F17" s="6"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>116</v>
+      </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="C20" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="9"/>
+      <c r="G20" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="10" t="s">
+        <v>144</v>
+      </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="9"/>
+      <c r="G21" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>145</v>
+      </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="9"/>
+      <c r="G22" s="10" t="s">
+        <v>150</v>
+      </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
@@ -1490,18 +1728,18 @@
       <c r="I25" s="9"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
@@ -1510,18 +1748,18 @@
       <c r="I26" s="9"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>104</v>
-      </c>
       <c r="D27" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
@@ -1530,27 +1768,31 @@
       <c r="I27" s="9"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="9"/>
+      <c r="G28" s="10" t="s">
+        <v>139</v>
+      </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>20</v>
       </c>
@@ -1558,50 +1800,58 @@
         <v>21</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="F29" s="6"/>
-      <c r="G29" s="9"/>
+      <c r="G29" s="10" t="s">
+        <v>140</v>
+      </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="F30" s="6"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="6"/>
@@ -1611,7 +1861,7 @@
       <c r="J31" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>